<commit_message>
Melhoria na aula de dplyr + tidyr. Melhorias margiais nas demais
</commit_message>
<xml_diff>
--- a/dados/simbioticos.xlsx
+++ b/dados/simbioticos.xlsx
@@ -381,10 +381,10 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B2">
-        <v>1.764782396007743</v>
+        <v>2.291101853716439</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -399,10 +399,10 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3">
-        <v>2.636980538723737</v>
+        <v>1.813875353205738</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -411,20 +411,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B4">
-        <v>2.002157054777778</v>
+        <v>2.337833915503559</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -435,10 +435,10 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B5">
-        <v>2.260264432486088</v>
+        <v>2.31475962183409</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -453,14 +453,14 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B6">
-        <v>2.133859937990451</v>
+        <v>2.160922553179256</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -471,28 +471,28 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B7">
-        <v>1.663348819173998</v>
+        <v>2.23316173857927</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cão</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8">
-        <v>1.950828339274434</v>
+        <v>1.846892395858312</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -510,7 +510,7 @@
         <v>44</v>
       </c>
       <c r="B9">
-        <v>1.762596331124318</v>
+        <v>1.761333439772967</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -525,14 +525,14 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B10">
-        <v>2.182043038679587</v>
+        <v>1.776794220975169</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cão</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -543,10 +543,10 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B11">
-        <v>1.967483664789418</v>
+        <v>1.847533227368614</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -555,20 +555,20 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B12">
-        <v>1.683602041875734</v>
+        <v>1.920674725903925</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -579,14 +579,14 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B13">
-        <v>2.014566104700579</v>
+        <v>1.767073144416038</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -597,10 +597,10 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B14">
-        <v>2.207786330581474</v>
+        <v>1.893064830607792</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -609,20 +609,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B15">
-        <v>1.887986622788802</v>
+        <v>1.880737281877479</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -633,14 +633,14 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B16">
-        <v>2.363557870109728</v>
+        <v>1.967930231372663</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Cão</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -654,7 +654,7 @@
         <v>38</v>
       </c>
       <c r="B17">
-        <v>1.942053577592279</v>
+        <v>2.584811023848867</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
@@ -663,16 +663,16 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18">
-        <v>2.373823932204024</v>
+        <v>1.987980829553026</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
@@ -687,10 +687,10 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B19">
-        <v>1.908531226360721</v>
+        <v>1.720510077599823</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
@@ -699,20 +699,20 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20">
-        <v>1.700026486214878</v>
+        <v>1.693192453402455</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Cão</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -726,7 +726,7 @@
         <v>38</v>
       </c>
       <c r="B21">
-        <v>2.041756945297248</v>
+        <v>2.139708245799606</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -735,20 +735,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22">
-        <v>1.577710089079681</v>
+        <v>1.530622695368917</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Cão</t>
+          <t>Gato</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -759,14 +759,14 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B23">
-        <v>2.174637242450899</v>
+        <v>2.378131809944018</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -777,10 +777,10 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="B24">
-        <v>2.264723640497692</v>
+        <v>2.473660434949607</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
@@ -789,16 +789,16 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B25">
-        <v>1.566000953455618</v>
+        <v>1.511908846581747</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -807,16 +807,16 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>1.918968703762069</v>
+        <v>1.542528890914957</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>H</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B27">
-        <v>1.994246642336019</v>
+        <v>2.379793990001072</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
@@ -843,34 +843,34 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B28">
-        <v>1.879556410417108</v>
+        <v>2.229671195325338</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B29">
-        <v>1.965877724350452</v>
+        <v>1.782895043764294</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
@@ -885,28 +885,28 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>1.694127868479277</v>
+        <v>2.477876120676674</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Gato</t>
+          <t>Cão</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B31">
-        <v>1.722385135929986</v>
+        <v>2.168616970564759</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>

</xml_diff>